<commit_message>
apresentação revisada e tópicos de fala adicionados
</commit_message>
<xml_diff>
--- a/Documentos/xml's/backlog.xlsx
+++ b/Documentos/xml's/backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\20201-3adsa-grupo1\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\20201-3adsa-grupo1\Documentos\xml's\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BF9BAA-7F40-403F-82D4-387390CC0A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAFA320-9318-4F4D-BC1E-0ADA45476A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="180">
   <si>
     <t>Proposto</t>
   </si>
@@ -489,15 +489,9 @@
     <t xml:space="preserve">Busca de localidades </t>
   </si>
   <si>
-    <t xml:space="preserve">Biblioteca de autocomplete </t>
-  </si>
-  <si>
     <t>Entregue</t>
   </si>
   <si>
-    <t>Projetado</t>
-  </si>
-  <si>
     <t>Passar API de Kotlin para JAVA</t>
   </si>
   <si>
@@ -571,6 +565,24 @@
   </si>
   <si>
     <t xml:space="preserve">Desenho de arquitetura de aplicação </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tela de Posts </t>
+  </si>
+  <si>
+    <t>Tela dedashboard do usuário</t>
+  </si>
+  <si>
+    <t>Diagrama de estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classe Post </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conexão com o  Heroku </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biblioteca Palces - API </t>
   </si>
 </sst>
 </file>
@@ -1385,6 +1397,10 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1454,10 +1470,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2309,10 +2321,10 @@
   <dimension ref="B1:V109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="F56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2363,22 +2375,22 @@
       <c r="U1" s="6"/>
     </row>
     <row r="2" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="68" t="s">
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="68"/>
+      <c r="P2" s="70"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="10"/>
       <c r="T2" s="11" t="s">
@@ -2387,40 +2399,40 @@
       <c r="U2" s="6"/>
     </row>
     <row r="3" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="70"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="72"/>
       <c r="Q3" s="1"/>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
     </row>
     <row r="4" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="80" t="s">
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="80"/>
+      <c r="P4" s="82"/>
       <c r="Q4" s="6"/>
       <c r="S4" s="12"/>
       <c r="T4" s="13"/>
@@ -2429,18 +2441,18 @@
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="D5" s="47"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="82"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="84"/>
       <c r="Q5" s="14"/>
       <c r="S5" s="12"/>
       <c r="T5" s="13"/>
@@ -2449,18 +2461,18 @@
     <row r="6" spans="2:22" s="15" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="16"/>
       <c r="D6" s="48"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="84"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="86"/>
       <c r="Q6" s="17"/>
       <c r="S6" s="18"/>
       <c r="T6" s="18"/>
@@ -2586,7 +2598,7 @@
       <c r="S9" s="49"/>
       <c r="T9" s="49"/>
       <c r="U9" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="2:22" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2618,7 +2630,7 @@
       <c r="S10" s="49"/>
       <c r="T10" s="49"/>
       <c r="U10" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="2:22" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -2650,7 +2662,7 @@
       <c r="S11" s="49"/>
       <c r="T11" s="49"/>
       <c r="U11" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="2:22" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2682,7 +2694,7 @@
       <c r="S12" s="49"/>
       <c r="T12" s="49"/>
       <c r="U12" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="2:22" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2714,7 +2726,7 @@
       <c r="S13" s="49"/>
       <c r="T13" s="49"/>
       <c r="U13" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="2:22" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -2746,7 +2758,7 @@
       <c r="S14" s="49"/>
       <c r="T14" s="49"/>
       <c r="U14" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="2:22" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2778,7 +2790,7 @@
       <c r="S15" s="49"/>
       <c r="T15" s="49"/>
       <c r="U15" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="2:22" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2810,7 +2822,7 @@
       <c r="S16" s="49"/>
       <c r="T16" s="49"/>
       <c r="U16" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -2842,7 +2854,7 @@
       <c r="S17" s="49"/>
       <c r="T17" s="49"/>
       <c r="U17" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2874,7 +2886,7 @@
       <c r="S18" s="49"/>
       <c r="T18" s="49"/>
       <c r="U18" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2906,7 +2918,7 @@
       <c r="S19" s="49"/>
       <c r="T19" s="49"/>
       <c r="U19" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -2938,7 +2950,7 @@
       <c r="S20" s="49"/>
       <c r="T20" s="49"/>
       <c r="U20" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2970,7 +2982,7 @@
       <c r="S21" s="49"/>
       <c r="T21" s="49"/>
       <c r="U21" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2980,11 +2992,15 @@
       <c r="C22" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="49"/>
+      <c r="D22" s="49" t="s">
+        <v>175</v>
+      </c>
       <c r="E22" s="49"/>
       <c r="F22" s="49"/>
       <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
+      <c r="H22" s="49" t="s">
+        <v>20</v>
+      </c>
       <c r="I22" s="49"/>
       <c r="J22" s="49"/>
       <c r="K22" s="49"/>
@@ -2997,7 +3013,9 @@
       <c r="R22" s="49"/>
       <c r="S22" s="49"/>
       <c r="T22" s="49"/>
-      <c r="U22" s="49"/>
+      <c r="U22" s="49" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26">
@@ -3006,11 +3024,15 @@
       <c r="C23" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="49"/>
+      <c r="D23" s="49" t="s">
+        <v>174</v>
+      </c>
       <c r="E23" s="49"/>
       <c r="F23" s="49"/>
       <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
+      <c r="H23" s="49" t="s">
+        <v>20</v>
+      </c>
       <c r="I23" s="49"/>
       <c r="J23" s="49"/>
       <c r="K23" s="49"/>
@@ -3023,7 +3045,9 @@
       <c r="R23" s="49"/>
       <c r="S23" s="49"/>
       <c r="T23" s="49"/>
-      <c r="U23" s="49"/>
+      <c r="U23" s="49" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="29">
@@ -3264,7 +3288,7 @@
       <c r="S32" s="49"/>
       <c r="T32" s="49"/>
       <c r="U32" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="2:21" s="28" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3328,7 +3352,7 @@
       <c r="S34" s="49"/>
       <c r="T34" s="49"/>
       <c r="U34" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3518,7 +3542,7 @@
       <c r="S41" s="49"/>
       <c r="T41" s="49"/>
       <c r="U41" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3550,7 +3574,7 @@
       <c r="S42" s="49"/>
       <c r="T42" s="49"/>
       <c r="U42" s="49" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3582,7 +3606,7 @@
       <c r="S43" s="49"/>
       <c r="T43" s="49"/>
       <c r="U43" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3614,7 +3638,7 @@
       <c r="S44" s="49"/>
       <c r="T44" s="49"/>
       <c r="U44" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3646,7 +3670,7 @@
       <c r="S45" s="49"/>
       <c r="T45" s="49"/>
       <c r="U45" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3678,7 +3702,7 @@
       <c r="S46" s="49"/>
       <c r="T46" s="49"/>
       <c r="U46" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3710,7 +3734,7 @@
       <c r="S47" s="49"/>
       <c r="T47" s="49"/>
       <c r="U47" s="49" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3742,7 +3766,7 @@
       <c r="S48" s="49"/>
       <c r="T48" s="49"/>
       <c r="U48" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3774,7 +3798,7 @@
       <c r="S49" s="49"/>
       <c r="T49" s="49"/>
       <c r="U49" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3806,7 +3830,7 @@
       <c r="S50" s="49"/>
       <c r="T50" s="49"/>
       <c r="U50" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3838,7 +3862,7 @@
       <c r="S51" s="49"/>
       <c r="T51" s="49"/>
       <c r="U51" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3870,7 +3894,7 @@
       <c r="S52" s="49"/>
       <c r="T52" s="49"/>
       <c r="U52" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3881,7 +3905,7 @@
         <v>40</v>
       </c>
       <c r="D53" s="49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E53" s="49"/>
       <c r="F53" s="49"/>
@@ -3901,7 +3925,9 @@
       <c r="R53" s="49"/>
       <c r="S53" s="49"/>
       <c r="T53" s="49"/>
-      <c r="U53" s="49"/>
+      <c r="U53" s="49" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="54" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="29">
@@ -3910,7 +3936,9 @@
       <c r="C54" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="49"/>
+      <c r="D54" s="49" t="s">
+        <v>176</v>
+      </c>
       <c r="E54" s="49"/>
       <c r="F54" s="49"/>
       <c r="G54" s="49"/>
@@ -3927,7 +3955,9 @@
       <c r="R54" s="49"/>
       <c r="S54" s="49"/>
       <c r="T54" s="49"/>
-      <c r="U54" s="49"/>
+      <c r="U54" s="49" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="26">
@@ -4066,7 +4096,7 @@
       <c r="C60" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D60" s="86"/>
+      <c r="D60" s="63"/>
       <c r="E60" s="49"/>
       <c r="F60" s="49"/>
       <c r="G60" s="49"/>
@@ -4112,7 +4142,7 @@
       <c r="S61" s="59"/>
       <c r="T61" s="59"/>
       <c r="U61" s="59" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -4123,7 +4153,7 @@
         <v>88</v>
       </c>
       <c r="D62" s="49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E62" s="49"/>
       <c r="F62" s="49"/>
@@ -4143,8 +4173,8 @@
       <c r="R62" s="49"/>
       <c r="S62" s="49"/>
       <c r="T62" s="49"/>
-      <c r="U62" s="49" t="s">
-        <v>0</v>
+      <c r="U62" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4154,8 +4184,8 @@
       <c r="C63" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="85" t="s">
-        <v>152</v>
+      <c r="D63" s="62" t="s">
+        <v>150</v>
       </c>
       <c r="E63" s="49"/>
       <c r="F63" s="49"/>
@@ -4175,7 +4205,9 @@
       <c r="R63" s="49"/>
       <c r="S63" s="49"/>
       <c r="T63" s="49"/>
-      <c r="U63" s="49"/>
+      <c r="U63" s="59" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="64" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="26">
@@ -4184,13 +4216,15 @@
       <c r="C64" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D64" s="85" t="s">
-        <v>153</v>
+      <c r="D64" s="62" t="s">
+        <v>151</v>
       </c>
       <c r="E64" s="49"/>
       <c r="F64" s="49"/>
       <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
+      <c r="H64" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I64" s="49"/>
       <c r="J64" s="49"/>
       <c r="K64" s="49"/>
@@ -4203,8 +4237,8 @@
       <c r="R64" s="49"/>
       <c r="S64" s="49"/>
       <c r="T64" s="49"/>
-      <c r="U64" s="49" t="s">
-        <v>0</v>
+      <c r="U64" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -4215,12 +4249,14 @@
         <v>91</v>
       </c>
       <c r="D65" s="49" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E65" s="49"/>
       <c r="F65" s="49"/>
       <c r="G65" s="49"/>
-      <c r="H65" s="49"/>
+      <c r="H65" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I65" s="49"/>
       <c r="J65" s="49"/>
       <c r="K65" s="49"/>
@@ -4233,8 +4269,8 @@
       <c r="R65" s="49"/>
       <c r="S65" s="49"/>
       <c r="T65" s="49"/>
-      <c r="U65" s="49" t="s">
-        <v>0</v>
+      <c r="U65" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4242,15 +4278,17 @@
         <v>59</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D66" s="49" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E66" s="49"/>
       <c r="F66" s="49"/>
       <c r="G66" s="49"/>
-      <c r="H66" s="49"/>
+      <c r="H66" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I66" s="49"/>
       <c r="J66" s="49"/>
       <c r="K66" s="49"/>
@@ -4263,22 +4301,26 @@
       <c r="R66" s="49"/>
       <c r="S66" s="49"/>
       <c r="T66" s="49"/>
-      <c r="U66" s="49"/>
+      <c r="U66" s="59" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="67" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="26">
         <v>60</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D67" s="49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E67" s="49"/>
       <c r="F67" s="49"/>
       <c r="G67" s="49"/>
-      <c r="H67" s="49"/>
+      <c r="H67" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I67" s="49"/>
       <c r="J67" s="49"/>
       <c r="K67" s="49"/>
@@ -4291,22 +4333,26 @@
       <c r="R67" s="49"/>
       <c r="S67" s="49"/>
       <c r="T67" s="49"/>
-      <c r="U67" s="49"/>
+      <c r="U67" s="59" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="68" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="26">
         <v>61</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D68" s="49" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E68" s="49"/>
       <c r="F68" s="49"/>
       <c r="G68" s="49"/>
-      <c r="H68" s="49"/>
+      <c r="H68" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I68" s="49"/>
       <c r="J68" s="49"/>
       <c r="K68" s="49"/>
@@ -4319,8 +4365,8 @@
       <c r="R68" s="49"/>
       <c r="S68" s="49"/>
       <c r="T68" s="49"/>
-      <c r="U68" s="49" t="s">
-        <v>0</v>
+      <c r="U68" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="69" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4328,15 +4374,17 @@
         <v>62</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D69" s="49" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E69" s="49"/>
       <c r="F69" s="49"/>
       <c r="G69" s="49"/>
-      <c r="H69" s="49"/>
+      <c r="H69" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I69" s="49"/>
       <c r="J69" s="49"/>
       <c r="K69" s="49"/>
@@ -4349,8 +4397,8 @@
       <c r="R69" s="49"/>
       <c r="S69" s="49"/>
       <c r="T69" s="49"/>
-      <c r="U69" s="49" t="s">
-        <v>0</v>
+      <c r="U69" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4358,15 +4406,17 @@
         <v>63</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D70" s="49" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E70" s="49"/>
       <c r="F70" s="49"/>
       <c r="G70" s="49"/>
-      <c r="H70" s="49"/>
+      <c r="H70" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I70" s="49"/>
       <c r="J70" s="49"/>
       <c r="K70" s="49"/>
@@ -4379,8 +4429,8 @@
       <c r="R70" s="49"/>
       <c r="S70" s="49"/>
       <c r="T70" s="49"/>
-      <c r="U70" s="49" t="s">
-        <v>0</v>
+      <c r="U70" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -4391,12 +4441,14 @@
         <v>92</v>
       </c>
       <c r="D71" s="49" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E71" s="49"/>
       <c r="F71" s="49"/>
       <c r="G71" s="49"/>
-      <c r="H71" s="49"/>
+      <c r="H71" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I71" s="49"/>
       <c r="J71" s="49"/>
       <c r="K71" s="49"/>
@@ -4409,8 +4461,8 @@
       <c r="R71" s="49"/>
       <c r="S71" s="49"/>
       <c r="T71" s="49"/>
-      <c r="U71" s="49" t="s">
-        <v>0</v>
+      <c r="U71" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4421,12 +4473,14 @@
         <v>93</v>
       </c>
       <c r="D72" s="49" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E72" s="49"/>
       <c r="F72" s="49"/>
       <c r="G72" s="49"/>
-      <c r="H72" s="49"/>
+      <c r="H72" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I72" s="49"/>
       <c r="J72" s="49"/>
       <c r="K72" s="49"/>
@@ -4439,22 +4493,26 @@
       <c r="R72" s="49"/>
       <c r="S72" s="49"/>
       <c r="T72" s="49"/>
-      <c r="U72" s="49"/>
+      <c r="U72" s="59" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="73" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="26">
         <v>66</v>
       </c>
       <c r="C73" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D73" s="49" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E73" s="49"/>
       <c r="F73" s="49"/>
       <c r="G73" s="49"/>
-      <c r="H73" s="49"/>
+      <c r="H73" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I73" s="49"/>
       <c r="J73" s="49"/>
       <c r="K73" s="49"/>
@@ -4467,22 +4525,26 @@
       <c r="R73" s="49"/>
       <c r="S73" s="49"/>
       <c r="T73" s="49"/>
-      <c r="U73" s="49"/>
+      <c r="U73" s="59" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="74" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="26">
         <v>67</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D74" s="49" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E74" s="49"/>
       <c r="F74" s="49"/>
       <c r="G74" s="49"/>
-      <c r="H74" s="49"/>
+      <c r="H74" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I74" s="49"/>
       <c r="J74" s="49"/>
       <c r="K74" s="49"/>
@@ -4495,7 +4557,9 @@
       <c r="R74" s="49"/>
       <c r="S74" s="49"/>
       <c r="T74" s="49"/>
-      <c r="U74" s="49"/>
+      <c r="U74" s="59" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="75" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="29">
@@ -4505,12 +4569,14 @@
         <v>94</v>
       </c>
       <c r="D75" s="49" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E75" s="49"/>
       <c r="F75" s="49"/>
       <c r="G75" s="49"/>
-      <c r="H75" s="49"/>
+      <c r="H75" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I75" s="49"/>
       <c r="J75" s="49"/>
       <c r="K75" s="49"/>
@@ -4523,8 +4589,8 @@
       <c r="R75" s="49"/>
       <c r="S75" s="49"/>
       <c r="T75" s="49"/>
-      <c r="U75" s="49" t="s">
-        <v>0</v>
+      <c r="U75" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4535,12 +4601,14 @@
         <v>95</v>
       </c>
       <c r="D76" s="49" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E76" s="49"/>
       <c r="F76" s="49"/>
       <c r="G76" s="49"/>
-      <c r="H76" s="49"/>
+      <c r="H76" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I76" s="49"/>
       <c r="J76" s="49"/>
       <c r="K76" s="49"/>
@@ -4553,8 +4621,8 @@
       <c r="R76" s="49"/>
       <c r="S76" s="49"/>
       <c r="T76" s="49"/>
-      <c r="U76" s="49" t="s">
-        <v>0</v>
+      <c r="U76" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -4564,13 +4632,15 @@
       <c r="C77" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D77" s="85" t="s">
-        <v>173</v>
+      <c r="D77" s="62" t="s">
+        <v>171</v>
       </c>
       <c r="E77" s="49"/>
       <c r="F77" s="49"/>
       <c r="G77" s="49"/>
-      <c r="H77" s="49"/>
+      <c r="H77" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I77" s="49"/>
       <c r="J77" s="49"/>
       <c r="K77" s="49"/>
@@ -4583,8 +4653,8 @@
       <c r="R77" s="49"/>
       <c r="S77" s="49"/>
       <c r="T77" s="49"/>
-      <c r="U77" s="49" t="s">
-        <v>0</v>
+      <c r="U77" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4594,11 +4664,15 @@
       <c r="C78" s="27">
         <v>4</v>
       </c>
-      <c r="D78" s="85"/>
+      <c r="D78" s="62" t="s">
+        <v>177</v>
+      </c>
       <c r="E78" s="49"/>
       <c r="F78" s="49"/>
       <c r="G78" s="49"/>
-      <c r="H78" s="49"/>
+      <c r="H78" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I78" s="49"/>
       <c r="J78" s="49"/>
       <c r="K78" s="49"/>
@@ -4611,8 +4685,8 @@
       <c r="R78" s="49"/>
       <c r="S78" s="49"/>
       <c r="T78" s="49"/>
-      <c r="U78" s="49" t="s">
-        <v>0</v>
+      <c r="U78" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4622,11 +4696,15 @@
       <c r="C79" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D79" s="85"/>
+      <c r="D79" s="62" t="s">
+        <v>178</v>
+      </c>
       <c r="E79" s="49"/>
       <c r="F79" s="49"/>
       <c r="G79" s="49"/>
-      <c r="H79" s="49"/>
+      <c r="H79" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I79" s="49"/>
       <c r="J79" s="49"/>
       <c r="K79" s="49"/>
@@ -4639,7 +4717,9 @@
       <c r="R79" s="49"/>
       <c r="S79" s="49"/>
       <c r="T79" s="49"/>
-      <c r="U79" s="49"/>
+      <c r="U79" s="59" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="80" spans="2:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="26">
@@ -4648,7 +4728,7 @@
       <c r="C80" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D80" s="85"/>
+      <c r="D80" s="62"/>
       <c r="E80" s="49"/>
       <c r="F80" s="49"/>
       <c r="G80" s="49"/>
@@ -5040,7 +5120,9 @@
       <c r="E94" s="49"/>
       <c r="F94" s="49"/>
       <c r="G94" s="49"/>
-      <c r="H94" s="49"/>
+      <c r="H94" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I94" s="49"/>
       <c r="J94" s="49"/>
       <c r="K94" s="49"/>
@@ -5065,12 +5147,14 @@
         <v>105</v>
       </c>
       <c r="D95" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E95" s="49"/>
       <c r="F95" s="49"/>
       <c r="G95" s="49"/>
-      <c r="H95" s="49"/>
+      <c r="H95" s="49" t="s">
+        <v>20</v>
+      </c>
       <c r="I95" s="49"/>
       <c r="J95" s="49"/>
       <c r="K95" s="49"/>
@@ -5100,7 +5184,9 @@
       <c r="E96" s="49"/>
       <c r="F96" s="49"/>
       <c r="G96" s="49"/>
-      <c r="H96" s="49"/>
+      <c r="H96" s="49" t="s">
+        <v>20</v>
+      </c>
       <c r="I96" s="49"/>
       <c r="J96" s="49"/>
       <c r="K96" s="49"/>
@@ -5130,7 +5216,9 @@
       <c r="E97" s="49"/>
       <c r="F97" s="49"/>
       <c r="G97" s="49"/>
-      <c r="H97" s="49"/>
+      <c r="H97" s="49" t="s">
+        <v>20</v>
+      </c>
       <c r="I97" s="49"/>
       <c r="J97" s="49"/>
       <c r="K97" s="49"/>
@@ -5155,12 +5243,14 @@
         <v>108</v>
       </c>
       <c r="D98" s="49" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="E98" s="49"/>
       <c r="F98" s="49"/>
       <c r="G98" s="49"/>
-      <c r="H98" s="49"/>
+      <c r="H98" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I98" s="49"/>
       <c r="J98" s="49"/>
       <c r="K98" s="49"/>
@@ -5416,7 +5506,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I40:I56 I8:I38 I61:I108" xr:uid="{CCF0E93B-E701-4254-9659-A3DB4D311139}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H25 H61:H70 H91:H92 H31:H38 H94:H98 H79:H82 H40:H53" xr:uid="{C6DF508E-944E-4154-8F9D-531F7223BA80}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H94:H98 H40:H53 H91:H92 H31:H38 H61:H82 H8:H25" xr:uid="{C6DF508E-944E-4154-8F9D-531F7223BA80}">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U108" xr:uid="{896C6ADC-A470-4136-B4BB-7A8530057896}">

</xml_diff>

<commit_message>
atualização do desenho de arquitetura
</commit_message>
<xml_diff>
--- a/Documentos/xml's/backlog.xlsx
+++ b/Documentos/xml's/backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\20201-3adsa-grupo1\Documentos\xml's\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAFA320-9318-4F4D-BC1E-0ADA45476A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82853F50-30F9-4A64-8F85-9ACF4C91A635}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="181">
   <si>
     <t>Proposto</t>
   </si>
@@ -582,7 +582,10 @@
     <t xml:space="preserve">Conexão com o  Heroku </t>
   </si>
   <si>
-    <t xml:space="preserve">Biblioteca Palces - API </t>
+    <t>Conexão com o Azure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biblioteca Places - API </t>
   </si>
 </sst>
 </file>
@@ -2321,10 +2324,10 @@
   <dimension ref="B1:V109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="F86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21:H23"/>
+      <selection pane="bottomRight" activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4728,11 +4731,15 @@
       <c r="C80" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D80" s="62"/>
+      <c r="D80" s="62" t="s">
+        <v>179</v>
+      </c>
       <c r="E80" s="49"/>
       <c r="F80" s="49"/>
       <c r="G80" s="49"/>
-      <c r="H80" s="49"/>
+      <c r="H80" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="I80" s="49"/>
       <c r="J80" s="49"/>
       <c r="K80" s="49"/>
@@ -4745,7 +4752,9 @@
       <c r="R80" s="49"/>
       <c r="S80" s="49"/>
       <c r="T80" s="49"/>
-      <c r="U80" s="49"/>
+      <c r="U80" s="49" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="2:21" s="28" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="29">
@@ -5243,7 +5252,7 @@
         <v>108</v>
       </c>
       <c r="D98" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E98" s="49"/>
       <c r="F98" s="49"/>
@@ -5506,7 +5515,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I40:I56 I8:I38 I61:I108" xr:uid="{CCF0E93B-E701-4254-9659-A3DB4D311139}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H94:H98 H40:H53 H91:H92 H31:H38 H61:H82 H8:H25" xr:uid="{C6DF508E-944E-4154-8F9D-531F7223BA80}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H94:H98 H40:H53 H91:H92 H31:H38 H8:H25 H61:H82" xr:uid="{C6DF508E-944E-4154-8F9D-531F7223BA80}">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U108" xr:uid="{896C6ADC-A470-4136-B4BB-7A8530057896}">

</xml_diff>